<commit_message>
bug guardado corregido y aumento ventana pureza_proporcion
</commit_message>
<xml_diff>
--- a/codigo/datasets/datasets_aumentados/logs/pcsmote/por_muestras/log_pcsmote_x_muestra_heart_D25_R25_Pentropia.xlsx
+++ b/codigo/datasets/datasets_aumentados/logs/pcsmote/por_muestras/log_pcsmote_x_muestra_heart_D25_R25_Pentropia.xlsx
@@ -435,7 +435,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Z68"/>
+  <dimension ref="A1:Z60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -653,17 +653,17 @@
         <v>1.637512517342308</v>
       </c>
       <c r="W2" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="X2" t="n">
-        <v>0.4239188491876604</v>
+        <v>0.4538824667597043</v>
       </c>
       <c r="Y2" t="n">
         <v>30</v>
       </c>
       <c r="Z2" t="inlineStr">
         <is>
-          <t>2025-10-27T20:44:53.660388</t>
+          <t>2025-10-29T23:40:24.423720</t>
         </is>
       </c>
     </row>
@@ -745,13 +745,17 @@
         <v>2.182639201208369</v>
       </c>
       <c r="W3" t="n">
-        <v>0</v>
-      </c>
-      <c r="X3" t="inlineStr"/>
-      <c r="Y3" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="X3" t="n">
+        <v>0.5616240759128834</v>
+      </c>
+      <c r="Y3" t="n">
+        <v>123</v>
+      </c>
       <c r="Z3" t="inlineStr">
         <is>
-          <t>2025-10-27T20:44:53.660388</t>
+          <t>2025-10-29T23:40:24.423720</t>
         </is>
       </c>
     </row>
@@ -833,17 +837,17 @@
         <v>2.628288156769919</v>
       </c>
       <c r="W4" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="X4" t="n">
-        <v>0.5542540693371891</v>
+        <v>0.4329311706285884</v>
       </c>
       <c r="Y4" t="n">
         <v>24</v>
       </c>
       <c r="Z4" t="inlineStr">
         <is>
-          <t>2025-10-27T20:44:53.660388</t>
+          <t>2025-10-29T23:40:24.423720</t>
         </is>
       </c>
     </row>
@@ -925,17 +929,17 @@
         <v>1.800964478621008</v>
       </c>
       <c r="W5" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="X5" t="n">
-        <v>0.4850311748982489</v>
+        <v>0.4153959819657586</v>
       </c>
       <c r="Y5" t="n">
-        <v>57</v>
+        <v>6</v>
       </c>
       <c r="Z5" t="inlineStr">
         <is>
-          <t>2025-10-27T20:44:53.660388</t>
+          <t>2025-10-29T23:40:24.423720</t>
         </is>
       </c>
     </row>
@@ -1027,7 +1031,7 @@
       </c>
       <c r="Z6" t="inlineStr">
         <is>
-          <t>2025-10-27T20:44:53.660388</t>
+          <t>2025-10-29T23:40:24.423720</t>
         </is>
       </c>
     </row>
@@ -1115,7 +1119,7 @@
       <c r="Y7" t="inlineStr"/>
       <c r="Z7" t="inlineStr">
         <is>
-          <t>2025-10-27T20:44:53.660388</t>
+          <t>2025-10-29T23:40:24.423720</t>
         </is>
       </c>
     </row>
@@ -1197,17 +1201,17 @@
         <v>2.615367358309021</v>
       </c>
       <c r="W8" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="X8" t="n">
-        <v>0.5544489538593315</v>
+        <v>0.5079682182603347</v>
       </c>
       <c r="Y8" t="n">
         <v>11</v>
       </c>
       <c r="Z8" t="inlineStr">
         <is>
-          <t>2025-10-27T20:44:53.660388</t>
+          <t>2025-10-29T23:40:24.423720</t>
         </is>
       </c>
     </row>
@@ -1299,7 +1303,7 @@
       </c>
       <c r="Z9" t="inlineStr">
         <is>
-          <t>2025-10-27T20:44:53.660388</t>
+          <t>2025-10-29T23:40:24.424719</t>
         </is>
       </c>
     </row>
@@ -1391,7 +1395,7 @@
       </c>
       <c r="Z10" t="inlineStr">
         <is>
-          <t>2025-10-27T20:44:53.660388</t>
+          <t>2025-10-29T23:40:24.424719</t>
         </is>
       </c>
     </row>
@@ -1483,7 +1487,7 @@
       </c>
       <c r="Z11" t="inlineStr">
         <is>
-          <t>2025-10-27T20:44:53.660388</t>
+          <t>2025-10-29T23:40:24.424719</t>
         </is>
       </c>
     </row>
@@ -1565,17 +1569,17 @@
         <v>2.351425882695806</v>
       </c>
       <c r="W12" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="X12" t="n">
-        <v>0.5413714687695235</v>
+        <v>0.5614880310328125</v>
       </c>
       <c r="Y12" t="n">
-        <v>4</v>
+        <v>120</v>
       </c>
       <c r="Z12" t="inlineStr">
         <is>
-          <t>2025-10-27T20:44:53.660388</t>
+          <t>2025-10-29T23:40:24.424719</t>
         </is>
       </c>
     </row>
@@ -1667,7 +1671,7 @@
       </c>
       <c r="Z13" t="inlineStr">
         <is>
-          <t>2025-10-27T20:44:53.660388</t>
+          <t>2025-10-29T23:40:24.424719</t>
         </is>
       </c>
     </row>
@@ -1749,13 +1753,17 @@
         <v>2.350674818698555</v>
       </c>
       <c r="W14" t="n">
-        <v>0</v>
-      </c>
-      <c r="X14" t="inlineStr"/>
-      <c r="Y14" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="X14" t="n">
+        <v>0.4062858371373469</v>
+      </c>
+      <c r="Y14" t="n">
+        <v>61</v>
+      </c>
       <c r="Z14" t="inlineStr">
         <is>
-          <t>2025-10-27T20:44:53.660388</t>
+          <t>2025-10-29T23:40:24.424719</t>
         </is>
       </c>
     </row>
@@ -1847,7 +1855,7 @@
       </c>
       <c r="Z15" t="inlineStr">
         <is>
-          <t>2025-10-27T20:44:53.660388</t>
+          <t>2025-10-29T23:40:24.424719</t>
         </is>
       </c>
     </row>
@@ -1929,17 +1937,17 @@
         <v>1.310501271630627</v>
       </c>
       <c r="W16" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="X16" t="n">
-        <v>0.4149101287359542</v>
+        <v>0.405083825348819</v>
       </c>
       <c r="Y16" t="n">
-        <v>71</v>
+        <v>21</v>
       </c>
       <c r="Z16" t="inlineStr">
         <is>
-          <t>2025-10-27T20:44:53.660388</t>
+          <t>2025-10-29T23:40:24.424719</t>
         </is>
       </c>
     </row>
@@ -2031,7 +2039,7 @@
       </c>
       <c r="Z17" t="inlineStr">
         <is>
-          <t>2025-10-27T20:44:53.660388</t>
+          <t>2025-10-29T23:40:24.425728</t>
         </is>
       </c>
     </row>
@@ -2123,7 +2131,7 @@
       </c>
       <c r="Z18" t="inlineStr">
         <is>
-          <t>2025-10-27T20:44:53.660388</t>
+          <t>2025-10-29T23:40:24.425728</t>
         </is>
       </c>
     </row>
@@ -2215,7 +2223,7 @@
       </c>
       <c r="Z19" t="inlineStr">
         <is>
-          <t>2025-10-27T20:44:53.660388</t>
+          <t>2025-10-29T23:40:24.425728</t>
         </is>
       </c>
     </row>
@@ -2303,7 +2311,7 @@
       <c r="Y20" t="inlineStr"/>
       <c r="Z20" t="inlineStr">
         <is>
-          <t>2025-10-27T20:44:53.660388</t>
+          <t>2025-10-29T23:40:24.425728</t>
         </is>
       </c>
     </row>
@@ -2391,7 +2399,7 @@
       <c r="Y21" t="inlineStr"/>
       <c r="Z21" t="inlineStr">
         <is>
-          <t>2025-10-27T20:44:53.660388</t>
+          <t>2025-10-29T23:40:24.425728</t>
         </is>
       </c>
     </row>
@@ -2483,7 +2491,7 @@
       </c>
       <c r="Z22" t="inlineStr">
         <is>
-          <t>2025-10-27T20:44:53.661388</t>
+          <t>2025-10-29T23:40:24.425728</t>
         </is>
       </c>
     </row>
@@ -2575,7 +2583,7 @@
       </c>
       <c r="Z23" t="inlineStr">
         <is>
-          <t>2025-10-27T20:44:53.661388</t>
+          <t>2025-10-29T23:40:24.425728</t>
         </is>
       </c>
     </row>
@@ -2667,7 +2675,7 @@
       </c>
       <c r="Z24" t="inlineStr">
         <is>
-          <t>2025-10-27T20:44:53.661388</t>
+          <t>2025-10-29T23:40:24.425728</t>
         </is>
       </c>
     </row>
@@ -2759,7 +2767,7 @@
       </c>
       <c r="Z25" t="inlineStr">
         <is>
-          <t>2025-10-27T20:44:53.661388</t>
+          <t>2025-10-29T23:40:24.426719</t>
         </is>
       </c>
     </row>
@@ -2841,17 +2849,17 @@
         <v>2.308100461078276</v>
       </c>
       <c r="W26" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="X26" t="n">
-        <v>0.5049549320516779</v>
+        <v>0.4705137712668338</v>
       </c>
       <c r="Y26" t="n">
-        <v>146</v>
+        <v>18</v>
       </c>
       <c r="Z26" t="inlineStr">
         <is>
-          <t>2025-10-27T20:44:53.661388</t>
+          <t>2025-10-29T23:40:24.426719</t>
         </is>
       </c>
     </row>
@@ -2933,17 +2941,17 @@
         <v>1.903279403849058</v>
       </c>
       <c r="W27" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="X27" t="n">
-        <v>0.4561869019374762</v>
+        <v>0.5541934359909122</v>
       </c>
       <c r="Y27" t="n">
         <v>123</v>
       </c>
       <c r="Z27" t="inlineStr">
         <is>
-          <t>2025-10-27T20:44:53.661388</t>
+          <t>2025-10-29T23:40:24.426719</t>
         </is>
       </c>
     </row>
@@ -3025,13 +3033,17 @@
         <v>2.375871974617221</v>
       </c>
       <c r="W28" t="n">
-        <v>0</v>
-      </c>
-      <c r="X28" t="inlineStr"/>
-      <c r="Y28" t="inlineStr"/>
+        <v>2</v>
+      </c>
+      <c r="X28" t="n">
+        <v>0.4969659942717967</v>
+      </c>
+      <c r="Y28" t="n">
+        <v>134</v>
+      </c>
       <c r="Z28" t="inlineStr">
         <is>
-          <t>2025-10-27T20:44:53.661388</t>
+          <t>2025-10-29T23:40:24.426719</t>
         </is>
       </c>
     </row>
@@ -3113,17 +3125,17 @@
         <v>2.312801572388097</v>
       </c>
       <c r="W29" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="X29" t="n">
-        <v>0.4281848449949526</v>
+        <v>0.4636006949943728</v>
       </c>
       <c r="Y29" t="n">
         <v>31</v>
       </c>
       <c r="Z29" t="inlineStr">
         <is>
-          <t>2025-10-27T20:44:53.661388</t>
+          <t>2025-10-29T23:40:24.426719</t>
         </is>
       </c>
     </row>
@@ -3205,17 +3217,17 @@
         <v>1.83165874525053</v>
       </c>
       <c r="W30" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="X30" t="n">
-        <v>0.4148089303468181</v>
+        <v>0.4641560129943472</v>
       </c>
       <c r="Y30" t="n">
         <v>108</v>
       </c>
       <c r="Z30" t="inlineStr">
         <is>
-          <t>2025-10-27T20:44:53.669336</t>
+          <t>2025-10-29T23:40:24.464051</t>
         </is>
       </c>
     </row>
@@ -3297,17 +3309,17 @@
         <v>3.344776669418398</v>
       </c>
       <c r="W31" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="X31" t="n">
-        <v>0.4127116700572048</v>
+        <v>0.4978905520555126</v>
       </c>
       <c r="Y31" t="n">
         <v>22</v>
       </c>
       <c r="Z31" t="inlineStr">
         <is>
-          <t>2025-10-27T20:44:53.669336</t>
+          <t>2025-10-29T23:40:24.464051</t>
         </is>
       </c>
     </row>
@@ -3389,17 +3401,17 @@
         <v>2.015717240620041</v>
       </c>
       <c r="W32" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="X32" t="n">
-        <v>0.4675230342807256</v>
+        <v>0.5290345580818899</v>
       </c>
       <c r="Y32" t="n">
         <v>80</v>
       </c>
       <c r="Z32" t="inlineStr">
         <is>
-          <t>2025-10-27T20:44:53.669336</t>
+          <t>2025-10-29T23:40:24.465051</t>
         </is>
       </c>
     </row>
@@ -3481,17 +3493,17 @@
         <v>2.036445016542462</v>
       </c>
       <c r="W33" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="X33" t="n">
-        <v>0.5721461166512687</v>
+        <v>0.5381875476204931</v>
       </c>
       <c r="Y33" t="n">
         <v>6</v>
       </c>
       <c r="Z33" t="inlineStr">
         <is>
-          <t>2025-10-27T20:44:53.669336</t>
+          <t>2025-10-29T23:40:24.465051</t>
         </is>
       </c>
     </row>
@@ -3573,17 +3585,17 @@
         <v>2.411746349972376</v>
       </c>
       <c r="W34" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="X34" t="n">
-        <v>0.4913069140965821</v>
+        <v>0.5966846281789686</v>
       </c>
       <c r="Y34" t="n">
         <v>91</v>
       </c>
       <c r="Z34" t="inlineStr">
         <is>
-          <t>2025-10-27T20:44:53.669336</t>
+          <t>2025-10-29T23:40:24.465051</t>
         </is>
       </c>
     </row>
@@ -3671,7 +3683,7 @@
       <c r="Y35" t="inlineStr"/>
       <c r="Z35" t="inlineStr">
         <is>
-          <t>2025-10-27T20:44:53.669336</t>
+          <t>2025-10-29T23:40:24.465051</t>
         </is>
       </c>
     </row>
@@ -3753,17 +3765,17 @@
         <v>2.342055414308382</v>
       </c>
       <c r="W36" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="X36" t="n">
-        <v>0.5037581243486732</v>
+        <v>0.4081550283109528</v>
       </c>
       <c r="Y36" t="n">
         <v>135</v>
       </c>
       <c r="Z36" t="inlineStr">
         <is>
-          <t>2025-10-27T20:44:53.669336</t>
+          <t>2025-10-29T23:40:24.466054</t>
         </is>
       </c>
     </row>
@@ -3851,7 +3863,7 @@
       <c r="Y37" t="inlineStr"/>
       <c r="Z37" t="inlineStr">
         <is>
-          <t>2025-10-27T20:44:53.669336</t>
+          <t>2025-10-29T23:40:24.466054</t>
         </is>
       </c>
     </row>
@@ -3933,17 +3945,17 @@
         <v>2.035697777445339</v>
       </c>
       <c r="W38" t="n">
+        <v>13</v>
+      </c>
+      <c r="X38" t="n">
+        <v>0.4739308912122809</v>
+      </c>
+      <c r="Y38" t="n">
         <v>11</v>
       </c>
-      <c r="X38" t="n">
-        <v>0.5021494605155131</v>
-      </c>
-      <c r="Y38" t="n">
-        <v>111</v>
-      </c>
       <c r="Z38" t="inlineStr">
         <is>
-          <t>2025-10-27T20:44:53.669336</t>
+          <t>2025-10-29T23:40:24.466054</t>
         </is>
       </c>
     </row>
@@ -4031,7 +4043,7 @@
       <c r="Y39" t="inlineStr"/>
       <c r="Z39" t="inlineStr">
         <is>
-          <t>2025-10-27T20:44:53.669336</t>
+          <t>2025-10-29T23:40:24.467052</t>
         </is>
       </c>
     </row>
@@ -4123,7 +4135,7 @@
       </c>
       <c r="Z40" t="inlineStr">
         <is>
-          <t>2025-10-27T20:44:53.669336</t>
+          <t>2025-10-29T23:40:24.467052</t>
         </is>
       </c>
     </row>
@@ -4205,17 +4217,17 @@
         <v>1.928557855300365</v>
       </c>
       <c r="W41" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="X41" t="n">
-        <v>0.4444215620941461</v>
+        <v>0.4727259204758588</v>
       </c>
       <c r="Y41" t="n">
         <v>118</v>
       </c>
       <c r="Z41" t="inlineStr">
         <is>
-          <t>2025-10-27T20:44:53.669336</t>
+          <t>2025-10-29T23:40:24.469055</t>
         </is>
       </c>
     </row>
@@ -4307,7 +4319,7 @@
       </c>
       <c r="Z42" t="inlineStr">
         <is>
-          <t>2025-10-27T20:44:53.669336</t>
+          <t>2025-10-29T23:40:24.469055</t>
         </is>
       </c>
     </row>
@@ -4399,7 +4411,7 @@
       </c>
       <c r="Z43" t="inlineStr">
         <is>
-          <t>2025-10-27T20:44:53.669336</t>
+          <t>2025-10-29T23:40:24.511505</t>
         </is>
       </c>
     </row>
@@ -4481,17 +4493,17 @@
         <v>3.711179640077895</v>
       </c>
       <c r="W44" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="X44" t="n">
-        <v>0.4899508266739531</v>
+        <v>0.4822074026636463</v>
       </c>
       <c r="Y44" t="n">
         <v>16</v>
       </c>
       <c r="Z44" t="inlineStr">
         <is>
-          <t>2025-10-27T20:44:53.669336</t>
+          <t>2025-10-29T23:40:24.512505</t>
         </is>
       </c>
     </row>
@@ -4573,17 +4585,17 @@
         <v>2.654491153386764</v>
       </c>
       <c r="W45" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="X45" t="n">
-        <v>0.476585374950758</v>
+        <v>0.42961738599068</v>
       </c>
       <c r="Y45" t="n">
         <v>116</v>
       </c>
       <c r="Z45" t="inlineStr">
         <is>
-          <t>2025-10-27T20:44:53.669336</t>
+          <t>2025-10-29T23:40:24.512505</t>
         </is>
       </c>
     </row>
@@ -4665,17 +4677,17 @@
         <v>3.326041139709015</v>
       </c>
       <c r="W46" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="X46" t="n">
-        <v>0.4278662908811752</v>
+        <v>0.5721461166512687</v>
       </c>
       <c r="Y46" t="n">
-        <v>152</v>
+        <v>16</v>
       </c>
       <c r="Z46" t="inlineStr">
         <is>
-          <t>2025-10-27T20:44:53.669336</t>
+          <t>2025-10-29T23:40:24.512505</t>
         </is>
       </c>
     </row>
@@ -4767,7 +4779,7 @@
       </c>
       <c r="Z47" t="inlineStr">
         <is>
-          <t>2025-10-27T20:44:53.669336</t>
+          <t>2025-10-29T23:40:24.512505</t>
         </is>
       </c>
     </row>
@@ -4859,7 +4871,7 @@
       </c>
       <c r="Z48" t="inlineStr">
         <is>
-          <t>2025-10-27T20:44:53.669336</t>
+          <t>2025-10-29T23:40:24.512505</t>
         </is>
       </c>
     </row>
@@ -4941,17 +4953,17 @@
         <v>2.140833741015508</v>
       </c>
       <c r="W49" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="X49" t="n">
-        <v>0.5389569866079409</v>
+        <v>0.4690142496053366</v>
       </c>
       <c r="Y49" t="n">
         <v>115</v>
       </c>
       <c r="Z49" t="inlineStr">
         <is>
-          <t>2025-10-27T20:44:53.669336</t>
+          <t>2025-10-29T23:40:24.512505</t>
         </is>
       </c>
     </row>
@@ -5033,17 +5045,17 @@
         <v>2.093666757006604</v>
       </c>
       <c r="W50" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="X50" t="n">
-        <v>0.5580351081062411</v>
+        <v>0.453356202855057</v>
       </c>
       <c r="Y50" t="n">
         <v>52</v>
       </c>
       <c r="Z50" t="inlineStr">
         <is>
-          <t>2025-10-27T20:44:53.669336</t>
+          <t>2025-10-29T23:40:24.512505</t>
         </is>
       </c>
     </row>
@@ -5125,17 +5137,17 @@
         <v>3.005590320299264</v>
       </c>
       <c r="W51" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="X51" t="n">
-        <v>0.4898901348276407</v>
+        <v>0.4444215620941461</v>
       </c>
       <c r="Y51" t="n">
         <v>17</v>
       </c>
       <c r="Z51" t="inlineStr">
         <is>
-          <t>2025-10-27T20:44:53.669336</t>
+          <t>2025-10-29T23:40:24.512505</t>
         </is>
       </c>
     </row>
@@ -5217,17 +5229,17 @@
         <v>2.656635308657509</v>
       </c>
       <c r="W52" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="X52" t="n">
-        <v>0.5829919351087561</v>
+        <v>0.5792182599846987</v>
       </c>
       <c r="Y52" t="n">
         <v>44</v>
       </c>
       <c r="Z52" t="inlineStr">
         <is>
-          <t>2025-10-27T20:44:53.669336</t>
+          <t>2025-10-29T23:40:24.512505</t>
         </is>
       </c>
     </row>
@@ -5315,7 +5327,7 @@
       <c r="Y53" t="inlineStr"/>
       <c r="Z53" t="inlineStr">
         <is>
-          <t>2025-10-27T20:44:53.669336</t>
+          <t>2025-10-29T23:40:24.512505</t>
         </is>
       </c>
     </row>
@@ -5407,7 +5419,7 @@
       </c>
       <c r="Z54" t="inlineStr">
         <is>
-          <t>2025-10-27T20:44:53.669336</t>
+          <t>2025-10-29T23:40:24.512505</t>
         </is>
       </c>
     </row>
@@ -5495,7 +5507,7 @@
       <c r="Y55" t="inlineStr"/>
       <c r="Z55" t="inlineStr">
         <is>
-          <t>2025-10-27T20:44:53.669336</t>
+          <t>2025-10-29T23:40:24.513505</t>
         </is>
       </c>
     </row>
@@ -5583,7 +5595,7 @@
       <c r="Y56" t="inlineStr"/>
       <c r="Z56" t="inlineStr">
         <is>
-          <t>2025-10-27T20:44:53.669336</t>
+          <t>2025-10-29T23:40:24.513505</t>
         </is>
       </c>
     </row>
@@ -5665,17 +5677,17 @@
         <v>2.101124475644301</v>
       </c>
       <c r="W57" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="X57" t="n">
-        <v>0.4403438404670793</v>
+        <v>0.5392608545679577</v>
       </c>
       <c r="Y57" t="n">
-        <v>151</v>
+        <v>118</v>
       </c>
       <c r="Z57" t="inlineStr">
         <is>
-          <t>2025-10-27T20:44:53.669336</t>
+          <t>2025-10-29T23:40:24.513505</t>
         </is>
       </c>
     </row>
@@ -5767,7 +5779,7 @@
       </c>
       <c r="Z58" t="inlineStr">
         <is>
-          <t>2025-10-27T20:44:53.669336</t>
+          <t>2025-10-29T23:40:24.513505</t>
         </is>
       </c>
     </row>
@@ -5849,17 +5861,17 @@
         <v>2.588880658408893</v>
       </c>
       <c r="W59" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="X59" t="n">
-        <v>0.4080867179076863</v>
+        <v>0.450783082786869</v>
       </c>
       <c r="Y59" t="n">
         <v>144</v>
       </c>
       <c r="Z59" t="inlineStr">
         <is>
-          <t>2025-10-27T20:44:53.682065</t>
+          <t>2025-10-29T23:40:24.513505</t>
         </is>
       </c>
     </row>
@@ -5941,726 +5953,22 @@
         <v>3.559080484587156</v>
       </c>
       <c r="W60" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="X60" t="n">
-        <v>0.4221781641623663</v>
+        <v>0.4646405864041511</v>
       </c>
       <c r="Y60" t="n">
         <v>22</v>
       </c>
       <c r="Z60" t="inlineStr">
         <is>
-          <t>2025-10-27T20:44:53.682135</t>
-        </is>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" t="inlineStr">
-        <is>
-          <t>heart</t>
-        </is>
-      </c>
-      <c r="B61" t="n">
-        <v>23</v>
-      </c>
-      <c r="C61" t="n">
-        <v>4</v>
-      </c>
-      <c r="D61" t="b">
-        <v>1</v>
-      </c>
-      <c r="E61" t="n">
-        <v>7</v>
-      </c>
-      <c r="F61" t="inlineStr"/>
-      <c r="G61" t="n">
-        <v>0.2857142857142857</v>
-      </c>
-      <c r="H61" t="n">
-        <v>0.5916727785823274</v>
-      </c>
-      <c r="I61" t="inlineStr">
-        <is>
-          <t>entropia</t>
-        </is>
-      </c>
-      <c r="J61" t="n">
-        <v>1</v>
-      </c>
-      <c r="K61" t="n">
-        <v>0.2857142857142857</v>
-      </c>
-      <c r="L61" t="n">
-        <v>0</v>
-      </c>
-      <c r="M61" t="inlineStr"/>
-      <c r="N61" t="b">
-        <v>1</v>
-      </c>
-      <c r="O61" t="b">
-        <v>1</v>
-      </c>
-      <c r="P61" t="inlineStr">
-        <is>
-          <t>[11, 107, 108, 50, 31, 6, 17]</t>
-        </is>
-      </c>
-      <c r="Q61" t="inlineStr">
-        <is>
-          <t>[0, 0, 0, 0, 0, 0, 0]</t>
-        </is>
-      </c>
-      <c r="R61" t="inlineStr">
-        <is>
-          <t>[2.0450439453125, 2.39786434173584, 2.5406486988067627, 2.7599363327026367, 2.763245105743408, 2.774099111557007, 2.8216850757598877]</t>
-        </is>
-      </c>
-      <c r="S61" t="inlineStr">
-        <is>
-          <t>[111, 122, 58, 49, 74, 29, 32]</t>
-        </is>
-      </c>
-      <c r="T61" t="inlineStr">
-        <is>
-          <t>[2.978161573410034, 4.0501909255981445, 4.2081098556518555, 4.714849472045898, 4.798360824584961, 5.375450611114502, 5.376267433166504]</t>
-        </is>
-      </c>
-      <c r="U61" t="n">
-        <v>2</v>
-      </c>
-      <c r="V61" t="n">
-        <v>2.469256530760287</v>
-      </c>
-      <c r="W61" t="n">
-        <v>0</v>
-      </c>
-      <c r="X61" t="inlineStr"/>
-      <c r="Y61" t="inlineStr"/>
-      <c r="Z61" t="inlineStr">
-        <is>
-          <t>2025-10-27T20:44:53.682592</t>
-        </is>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" t="inlineStr">
-        <is>
-          <t>heart</t>
-        </is>
-      </c>
-      <c r="B62" t="n">
-        <v>29</v>
-      </c>
-      <c r="C62" t="n">
-        <v>4</v>
-      </c>
-      <c r="D62" t="b">
-        <v>1</v>
-      </c>
-      <c r="E62" t="n">
-        <v>7</v>
-      </c>
-      <c r="F62" t="inlineStr"/>
-      <c r="G62" t="n">
-        <v>0.2857142857142857</v>
-      </c>
-      <c r="H62" t="n">
-        <v>0.5916727785823274</v>
-      </c>
-      <c r="I62" t="inlineStr">
-        <is>
-          <t>entropia</t>
-        </is>
-      </c>
-      <c r="J62" t="n">
-        <v>0.8571428571428571</v>
-      </c>
-      <c r="K62" t="n">
-        <v>0.2857142857142857</v>
-      </c>
-      <c r="L62" t="n">
-        <v>0.5916727785823274</v>
-      </c>
-      <c r="M62" t="inlineStr"/>
-      <c r="N62" t="b">
-        <v>1</v>
-      </c>
-      <c r="O62" t="b">
-        <v>1</v>
-      </c>
-      <c r="P62" t="inlineStr">
-        <is>
-          <t>[0, 122, 50, 20, 100, 149, 108]</t>
-        </is>
-      </c>
-      <c r="Q62" t="inlineStr">
-        <is>
-          <t>[0, 1, 0, 0, 0, 0, 0]</t>
-        </is>
-      </c>
-      <c r="R62" t="inlineStr">
-        <is>
-          <t>[3.3233187198638916, 4.059734344482422, 4.167458534240723, 4.20436429977417, 4.278962135314941, 4.5680131912231445, 4.604304790496826]</t>
-        </is>
-      </c>
-      <c r="S62" t="inlineStr">
-        <is>
-          <t>[122, 49, 111, 32, 23, 58, 74]</t>
-        </is>
-      </c>
-      <c r="T62" t="inlineStr">
-        <is>
-          <t>[4.059734344482422, 4.712945938110352, 4.923409938812256, 5.225722312927246, 5.375450611114502, 6.480259418487549, 7.0887932777404785]</t>
-        </is>
-      </c>
-      <c r="U62" t="n">
-        <v>2</v>
-      </c>
-      <c r="V62" t="n">
-        <v>4.113596337415536</v>
-      </c>
-      <c r="W62" t="n">
-        <v>0</v>
-      </c>
-      <c r="X62" t="inlineStr"/>
-      <c r="Y62" t="inlineStr"/>
-      <c r="Z62" t="inlineStr">
-        <is>
-          <t>2025-10-27T20:44:53.682592</t>
-        </is>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" t="inlineStr">
-        <is>
-          <t>heart</t>
-        </is>
-      </c>
-      <c r="B63" t="n">
-        <v>32</v>
-      </c>
-      <c r="C63" t="n">
-        <v>4</v>
-      </c>
-      <c r="D63" t="b">
-        <v>0</v>
-      </c>
-      <c r="E63" t="n">
-        <v>7</v>
-      </c>
-      <c r="F63" t="inlineStr"/>
-      <c r="G63" t="n">
-        <v>0.2857142857142857</v>
-      </c>
-      <c r="H63" t="n">
-        <v>0.5916727785823274</v>
-      </c>
-      <c r="I63" t="inlineStr">
-        <is>
-          <t>entropia</t>
-        </is>
-      </c>
-      <c r="J63" t="n">
-        <v>0.7142857142857143</v>
-      </c>
-      <c r="K63" t="n">
-        <v>0.2857142857142857</v>
-      </c>
-      <c r="L63" t="n">
-        <v>0.8631205685666311</v>
-      </c>
-      <c r="M63" t="inlineStr"/>
-      <c r="N63" t="b">
-        <v>0</v>
-      </c>
-      <c r="O63" t="b">
-        <v>1</v>
-      </c>
-      <c r="P63" t="inlineStr">
-        <is>
-          <t>[152, 111, 100, 50, 3, 16, 49]</t>
-        </is>
-      </c>
-      <c r="Q63" t="inlineStr">
-        <is>
-          <t>[0, 1, 0, 0, 0, 0, 1]</t>
-        </is>
-      </c>
-      <c r="R63" t="inlineStr">
-        <is>
-          <t>[3.581364870071411, 3.782494068145752, 3.862605571746826, 3.9095888137817383, 3.9325404167175293, 3.952988386154175, 3.967590808868408]</t>
-        </is>
-      </c>
-      <c r="S63" t="inlineStr">
-        <is>
-          <t>[111, 49, 29, 23, 122, 58, 74]</t>
-        </is>
-      </c>
-      <c r="T63" t="inlineStr">
-        <is>
-          <t>[3.782494068145752, 3.967590808868408, 5.225722312927246, 5.376267433166504, 5.447623252868652, 5.880111217498779, 6.302395343780518]</t>
-        </is>
-      </c>
-      <c r="U63" t="n">
-        <v>2</v>
-      </c>
-      <c r="V63" t="n">
-        <v>3.822549829585008</v>
-      </c>
-      <c r="W63" t="n">
-        <v>0</v>
-      </c>
-      <c r="X63" t="inlineStr"/>
-      <c r="Y63" t="inlineStr"/>
-      <c r="Z63" t="inlineStr">
-        <is>
-          <t>2025-10-27T20:44:53.682592</t>
-        </is>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" t="inlineStr">
-        <is>
-          <t>heart</t>
-        </is>
-      </c>
-      <c r="B64" t="n">
-        <v>49</v>
-      </c>
-      <c r="C64" t="n">
-        <v>4</v>
-      </c>
-      <c r="D64" t="b">
-        <v>1</v>
-      </c>
-      <c r="E64" t="n">
-        <v>7</v>
-      </c>
-      <c r="F64" t="inlineStr"/>
-      <c r="G64" t="n">
-        <v>0.2857142857142857</v>
-      </c>
-      <c r="H64" t="n">
-        <v>0.5916727785823274</v>
-      </c>
-      <c r="I64" t="inlineStr">
-        <is>
-          <t>entropia</t>
-        </is>
-      </c>
-      <c r="J64" t="n">
-        <v>0.8571428571428571</v>
-      </c>
-      <c r="K64" t="n">
-        <v>0.2857142857142857</v>
-      </c>
-      <c r="L64" t="n">
-        <v>0.5916727785823274</v>
-      </c>
-      <c r="M64" t="inlineStr"/>
-      <c r="N64" t="b">
-        <v>1</v>
-      </c>
-      <c r="O64" t="b">
-        <v>1</v>
-      </c>
-      <c r="P64" t="inlineStr">
-        <is>
-          <t>[0, 111, 100, 57, 108, 11, 50]</t>
-        </is>
-      </c>
-      <c r="Q64" t="inlineStr">
-        <is>
-          <t>[0, 1, 0, 0, 0, 0, 0]</t>
-        </is>
-      </c>
-      <c r="R64" t="inlineStr">
-        <is>
-          <t>[2.7044990062713623, 2.744593620300293, 3.03739595413208, 3.6008496284484863, 3.601428508758545, 3.613584280014038, 3.7613816261291504]</t>
-        </is>
-      </c>
-      <c r="S64" t="inlineStr">
-        <is>
-          <t>[111, 32, 29, 23, 58, 122, 74]</t>
-        </is>
-      </c>
-      <c r="T64" t="inlineStr">
-        <is>
-          <t>[2.744593620300293, 3.967590808868408, 4.712945938110352, 4.714849472045898, 5.023791790008545, 5.143283843994141, 5.44774866104126]</t>
-        </is>
-      </c>
-      <c r="U64" t="n">
-        <v>2</v>
-      </c>
-      <c r="V64" t="n">
-        <v>2.890994812564799</v>
-      </c>
-      <c r="W64" t="n">
-        <v>0</v>
-      </c>
-      <c r="X64" t="inlineStr"/>
-      <c r="Y64" t="inlineStr"/>
-      <c r="Z64" t="inlineStr">
-        <is>
-          <t>2025-10-27T20:44:53.682592</t>
-        </is>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" t="inlineStr">
-        <is>
-          <t>heart</t>
-        </is>
-      </c>
-      <c r="B65" t="n">
-        <v>58</v>
-      </c>
-      <c r="C65" t="n">
-        <v>4</v>
-      </c>
-      <c r="D65" t="b">
-        <v>1</v>
-      </c>
-      <c r="E65" t="n">
-        <v>7</v>
-      </c>
-      <c r="F65" t="inlineStr"/>
-      <c r="G65" t="n">
-        <v>0.2857142857142857</v>
-      </c>
-      <c r="H65" t="n">
-        <v>0.5916727785823274</v>
-      </c>
-      <c r="I65" t="inlineStr">
-        <is>
-          <t>entropia</t>
-        </is>
-      </c>
-      <c r="J65" t="n">
-        <v>0.8571428571428571</v>
-      </c>
-      <c r="K65" t="n">
-        <v>0.2857142857142857</v>
-      </c>
-      <c r="L65" t="n">
-        <v>0.5916727785823274</v>
-      </c>
-      <c r="M65" t="inlineStr"/>
-      <c r="N65" t="b">
-        <v>1</v>
-      </c>
-      <c r="O65" t="b">
-        <v>1</v>
-      </c>
-      <c r="P65" t="inlineStr">
-        <is>
-          <t>[116, 125, 6, 30, 144, 111, 80]</t>
-        </is>
-      </c>
-      <c r="Q65" t="inlineStr">
-        <is>
-          <t>[0, 0, 0, 0, 0, 1, 0]</t>
-        </is>
-      </c>
-      <c r="R65" t="inlineStr">
-        <is>
-          <t>[2.321561098098755, 2.989548683166504, 2.9944894313812256, 3.028784990310669, 3.167263984680176, 3.3404667377471924, 3.3468122482299805]</t>
-        </is>
-      </c>
-      <c r="S65" t="inlineStr">
-        <is>
-          <t>[111, 74, 23, 49, 122, 32, 29]</t>
-        </is>
-      </c>
-      <c r="T65" t="inlineStr">
-        <is>
-          <t>[3.3404667377471924, 3.7469117641448975, 4.2081098556518555, 5.023791790008545, 5.170320510864258, 5.880111217498779, 6.480259418487549]</t>
-        </is>
-      </c>
-      <c r="U65" t="n">
-        <v>2</v>
-      </c>
-      <c r="V65" t="n">
-        <v>2.99201913047313</v>
-      </c>
-      <c r="W65" t="n">
-        <v>0</v>
-      </c>
-      <c r="X65" t="inlineStr"/>
-      <c r="Y65" t="inlineStr"/>
-      <c r="Z65" t="inlineStr">
-        <is>
-          <t>2025-10-27T20:44:53.682592</t>
-        </is>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" t="inlineStr">
-        <is>
-          <t>heart</t>
-        </is>
-      </c>
-      <c r="B66" t="n">
-        <v>74</v>
-      </c>
-      <c r="C66" t="n">
-        <v>4</v>
-      </c>
-      <c r="D66" t="b">
-        <v>1</v>
-      </c>
-      <c r="E66" t="n">
-        <v>7</v>
-      </c>
-      <c r="F66" t="inlineStr"/>
-      <c r="G66" t="n">
-        <v>0.2857142857142857</v>
-      </c>
-      <c r="H66" t="n">
-        <v>0.5916727785823274</v>
-      </c>
-      <c r="I66" t="inlineStr">
-        <is>
-          <t>entropia</t>
-        </is>
-      </c>
-      <c r="J66" t="n">
-        <v>1</v>
-      </c>
-      <c r="K66" t="n">
-        <v>0.2857142857142857</v>
-      </c>
-      <c r="L66" t="n">
-        <v>0</v>
-      </c>
-      <c r="M66" t="inlineStr"/>
-      <c r="N66" t="b">
-        <v>1</v>
-      </c>
-      <c r="O66" t="b">
-        <v>1</v>
-      </c>
-      <c r="P66" t="inlineStr">
-        <is>
-          <t>[15, 151, 26, 116, 134, 79, 6]</t>
-        </is>
-      </c>
-      <c r="Q66" t="inlineStr">
-        <is>
-          <t>[0, 0, 0, 0, 0, 0, 0]</t>
-        </is>
-      </c>
-      <c r="R66" t="inlineStr">
-        <is>
-          <t>[2.989654302597046, 3.279348850250244, 3.4450466632843018, 3.4723429679870605, 3.5377962589263916, 3.582503318786621, 3.678356170654297]</t>
-        </is>
-      </c>
-      <c r="S66" t="inlineStr">
-        <is>
-          <t>[58, 111, 23, 49, 122, 32, 29]</t>
-        </is>
-      </c>
-      <c r="T66" t="inlineStr">
-        <is>
-          <t>[3.7469117641448975, 4.177338600158691, 4.798360824584961, 5.44774866104126, 5.6261515617370605, 6.302395343780518, 7.0887932777404785]</t>
-        </is>
-      </c>
-      <c r="U66" t="n">
-        <v>2</v>
-      </c>
-      <c r="V66" t="n">
-        <v>3.362197711240765</v>
-      </c>
-      <c r="W66" t="n">
-        <v>0</v>
-      </c>
-      <c r="X66" t="inlineStr"/>
-      <c r="Y66" t="inlineStr"/>
-      <c r="Z66" t="inlineStr">
-        <is>
-          <t>2025-10-27T20:44:53.682592</t>
-        </is>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" t="inlineStr">
-        <is>
-          <t>heart</t>
-        </is>
-      </c>
-      <c r="B67" t="n">
-        <v>111</v>
-      </c>
-      <c r="C67" t="n">
-        <v>4</v>
-      </c>
-      <c r="D67" t="b">
-        <v>1</v>
-      </c>
-      <c r="E67" t="n">
-        <v>7</v>
-      </c>
-      <c r="F67" t="inlineStr"/>
-      <c r="G67" t="n">
-        <v>0.2857142857142857</v>
-      </c>
-      <c r="H67" t="n">
-        <v>0.5916727785823274</v>
-      </c>
-      <c r="I67" t="inlineStr">
-        <is>
-          <t>entropia</t>
-        </is>
-      </c>
-      <c r="J67" t="n">
-        <v>1</v>
-      </c>
-      <c r="K67" t="n">
-        <v>0.2857142857142857</v>
-      </c>
-      <c r="L67" t="n">
-        <v>0</v>
-      </c>
-      <c r="M67" t="inlineStr"/>
-      <c r="N67" t="b">
-        <v>1</v>
-      </c>
-      <c r="O67" t="b">
-        <v>1</v>
-      </c>
-      <c r="P67" t="inlineStr">
-        <is>
-          <t>[108, 11, 100, 50, 26, 30, 57]</t>
-        </is>
-      </c>
-      <c r="Q67" t="inlineStr">
-        <is>
-          <t>[0, 0, 0, 0, 0, 0, 0]</t>
-        </is>
-      </c>
-      <c r="R67" t="inlineStr">
-        <is>
-          <t>[1.7137212753295898, 1.8753184080123901, 1.9820659160614014, 2.4990010261535645, 2.7067956924438477, 2.70947003364563, 2.71624755859375]</t>
-        </is>
-      </c>
-      <c r="S67" t="inlineStr">
-        <is>
-          <t>[49, 23, 58, 32, 122, 74, 29]</t>
-        </is>
-      </c>
-      <c r="T67" t="inlineStr">
-        <is>
-          <t>[2.744593620300293, 2.978161573410034, 3.3404667377471924, 3.782494068145752, 4.119991302490234, 4.177338600158691, 4.923409938812256]</t>
-        </is>
-      </c>
-      <c r="U67" t="n">
-        <v>2</v>
-      </c>
-      <c r="V67" t="n">
-        <v>1.928692209533841</v>
-      </c>
-      <c r="W67" t="n">
-        <v>0</v>
-      </c>
-      <c r="X67" t="inlineStr"/>
-      <c r="Y67" t="inlineStr"/>
-      <c r="Z67" t="inlineStr">
-        <is>
-          <t>2025-10-27T20:44:53.682592</t>
-        </is>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" t="inlineStr">
-        <is>
-          <t>heart</t>
-        </is>
-      </c>
-      <c r="B68" t="n">
-        <v>122</v>
-      </c>
-      <c r="C68" t="n">
-        <v>4</v>
-      </c>
-      <c r="D68" t="b">
-        <v>1</v>
-      </c>
-      <c r="E68" t="n">
-        <v>7</v>
-      </c>
-      <c r="F68" t="inlineStr"/>
-      <c r="G68" t="n">
-        <v>0.2857142857142857</v>
-      </c>
-      <c r="H68" t="n">
-        <v>0.5916727785823274</v>
-      </c>
-      <c r="I68" t="inlineStr">
-        <is>
-          <t>entropia</t>
-        </is>
-      </c>
-      <c r="J68" t="n">
-        <v>1</v>
-      </c>
-      <c r="K68" t="n">
-        <v>0.2857142857142857</v>
-      </c>
-      <c r="L68" t="n">
-        <v>0</v>
-      </c>
-      <c r="M68" t="inlineStr"/>
-      <c r="N68" t="b">
-        <v>1</v>
-      </c>
-      <c r="O68" t="b">
-        <v>1</v>
-      </c>
-      <c r="P68" t="inlineStr">
-        <is>
-          <t>[143, 108, 100, 118, 151, 20, 30]</t>
-        </is>
-      </c>
-      <c r="Q68" t="inlineStr">
-        <is>
-          <t>[0, 0, 0, 0, 0, 0, 0]</t>
-        </is>
-      </c>
-      <c r="R68" t="inlineStr">
-        <is>
-          <t>[3.4728429317474365, 3.7831006050109863, 3.8177778720855713, 3.835824966430664, 3.876563787460327, 3.8958423137664795, 4.041891574859619]</t>
-        </is>
-      </c>
-      <c r="S68" t="inlineStr">
-        <is>
-          <t>[23, 29, 111, 49, 58, 32, 74]</t>
-        </is>
-      </c>
-      <c r="T68" t="inlineStr">
-        <is>
-          <t>[4.0501909255981445, 4.059734344482422, 4.119991302490234, 5.143283843994141, 5.170320510864258, 5.447623252868652, 5.6261515617370605]</t>
-        </is>
-      </c>
-      <c r="U68" t="n">
-        <v>2</v>
-      </c>
-      <c r="V68" t="n">
-        <v>3.80043923668247</v>
-      </c>
-      <c r="W68" t="n">
-        <v>0</v>
-      </c>
-      <c r="X68" t="inlineStr"/>
-      <c r="Y68" t="inlineStr"/>
-      <c r="Z68" t="inlineStr">
-        <is>
-          <t>2025-10-27T20:44:53.682592</t>
+          <t>2025-10-29T23:40:24.513505</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:Z68">
+  <conditionalFormatting sqref="A2:Z60">
     <cfRule type="expression" priority="1" dxfId="0">
       <formula>=$D2=FALSE</formula>
     </cfRule>

</xml_diff>